<commit_message>
comit 13 de febrero
</commit_message>
<xml_diff>
--- a/BD paper/catalogos/waveform_1-2.9_filtered.xlsx
+++ b/BD paper/catalogos/waveform_1-2.9_filtered.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P126"/>
+  <dimension ref="A1:T126"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -518,6 +518,26 @@
           <t>Inicio estación más cercana 5</t>
         </is>
       </c>
+      <c r="Q1" s="1" t="inlineStr">
+        <is>
+          <t>Estación más cercana 6</t>
+        </is>
+      </c>
+      <c r="R1" s="1" t="inlineStr">
+        <is>
+          <t>Estación más cercana 7</t>
+        </is>
+      </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Inicio estación más cercana 6</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Inicio estación más cercana 7</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -590,6 +610,26 @@
           <t>2014-01-08T07:13:19</t>
         </is>
       </c>
+      <c r="Q2" t="inlineStr">
+        <is>
+          <t>PB15</t>
+        </is>
+      </c>
+      <c r="R2" t="inlineStr">
+        <is>
+          <t>PB05</t>
+        </is>
+      </c>
+      <c r="S2" t="inlineStr">
+        <is>
+          <t>2014-01-08T07:13:23</t>
+        </is>
+      </c>
+      <c r="T2" t="inlineStr">
+        <is>
+          <t>2014-01-08T07:13:24</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -662,6 +702,26 @@
           <t>2014-01-08T11:07:12</t>
         </is>
       </c>
+      <c r="Q3" t="inlineStr">
+        <is>
+          <t>PB01</t>
+        </is>
+      </c>
+      <c r="R3" t="inlineStr">
+        <is>
+          <t>PB03</t>
+        </is>
+      </c>
+      <c r="S3" t="inlineStr">
+        <is>
+          <t>2014-01-08T11:07:12</t>
+        </is>
+      </c>
+      <c r="T3" t="inlineStr">
+        <is>
+          <t>2014-01-08T11:07:13</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -734,6 +794,26 @@
           <t>2014-01-18T01:30:05</t>
         </is>
       </c>
+      <c r="Q4" t="inlineStr">
+        <is>
+          <t>PB07</t>
+        </is>
+      </c>
+      <c r="R4" t="inlineStr">
+        <is>
+          <t>PB10</t>
+        </is>
+      </c>
+      <c r="S4" t="inlineStr">
+        <is>
+          <t>2014-01-18T01:30:08</t>
+        </is>
+      </c>
+      <c r="T4" t="inlineStr">
+        <is>
+          <t>2014-01-18T01:30:09</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -806,6 +886,26 @@
           <t>2014-01-23T02:34:48</t>
         </is>
       </c>
+      <c r="Q5" t="inlineStr">
+        <is>
+          <t>PB09</t>
+        </is>
+      </c>
+      <c r="R5" t="inlineStr">
+        <is>
+          <t>PATCX</t>
+        </is>
+      </c>
+      <c r="S5" t="inlineStr">
+        <is>
+          <t>2014-01-23T02:34:48</t>
+        </is>
+      </c>
+      <c r="T5" t="inlineStr">
+        <is>
+          <t>2014-01-23T02:34:49</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -878,6 +978,26 @@
           <t>2014-02-03T12:36:45</t>
         </is>
       </c>
+      <c r="Q6" t="inlineStr">
+        <is>
+          <t>AC06</t>
+        </is>
+      </c>
+      <c r="R6" t="inlineStr">
+        <is>
+          <t>AC07</t>
+        </is>
+      </c>
+      <c r="S6" t="inlineStr">
+        <is>
+          <t>2014-02-03T12:36:46</t>
+        </is>
+      </c>
+      <c r="T6" t="inlineStr">
+        <is>
+          <t>2014-02-03T12:36:46</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -950,6 +1070,26 @@
           <t>2014-02-07T18:35:33</t>
         </is>
       </c>
+      <c r="Q7" t="inlineStr">
+        <is>
+          <t>TA01</t>
+        </is>
+      </c>
+      <c r="R7" t="inlineStr">
+        <is>
+          <t>HMBCX</t>
+        </is>
+      </c>
+      <c r="S7" t="inlineStr">
+        <is>
+          <t>2014-02-07T18:35:34</t>
+        </is>
+      </c>
+      <c r="T7" t="inlineStr">
+        <is>
+          <t>2014-02-07T18:35:34</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -1022,6 +1162,26 @@
           <t>2014-02-21T18:17:38</t>
         </is>
       </c>
+      <c r="Q8" t="inlineStr">
+        <is>
+          <t>PB06</t>
+        </is>
+      </c>
+      <c r="R8" t="inlineStr">
+        <is>
+          <t>PB02</t>
+        </is>
+      </c>
+      <c r="S8" t="inlineStr">
+        <is>
+          <t>2014-02-21T18:17:40</t>
+        </is>
+      </c>
+      <c r="T8" t="inlineStr">
+        <is>
+          <t>2014-02-21T18:17:43</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1094,6 +1254,26 @@
           <t>2014-02-25T00:03:15</t>
         </is>
       </c>
+      <c r="Q9" t="inlineStr">
+        <is>
+          <t>TA01</t>
+        </is>
+      </c>
+      <c r="R9" t="inlineStr">
+        <is>
+          <t>MNMCX</t>
+        </is>
+      </c>
+      <c r="S9" t="inlineStr">
+        <is>
+          <t>2014-02-25T00:03:17</t>
+        </is>
+      </c>
+      <c r="T9" t="inlineStr">
+        <is>
+          <t>2014-02-25T00:03:18</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1166,6 +1346,26 @@
           <t>2014-02-28T20:36:54</t>
         </is>
       </c>
+      <c r="Q10" t="inlineStr">
+        <is>
+          <t>AC01</t>
+        </is>
+      </c>
+      <c r="R10" t="inlineStr">
+        <is>
+          <t>PB15</t>
+        </is>
+      </c>
+      <c r="S10" t="inlineStr">
+        <is>
+          <t>2014-02-28T20:36:55</t>
+        </is>
+      </c>
+      <c r="T10" t="inlineStr">
+        <is>
+          <t>2014-02-28T20:36:59</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1238,6 +1438,26 @@
           <t>2014-03-17T15:49:10</t>
         </is>
       </c>
+      <c r="Q11" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R11" t="inlineStr">
+        <is>
+          <t>PX02</t>
+        </is>
+      </c>
+      <c r="S11" t="inlineStr">
+        <is>
+          <t>2014-03-17T15:49:11</t>
+        </is>
+      </c>
+      <c r="T11" t="inlineStr">
+        <is>
+          <t>2014-03-17T15:49:11</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1310,6 +1530,26 @@
           <t>2014-03-18T03:19:51</t>
         </is>
       </c>
+      <c r="Q12" t="inlineStr">
+        <is>
+          <t>PATCX</t>
+        </is>
+      </c>
+      <c r="R12" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="S12" t="inlineStr">
+        <is>
+          <t>2014-03-18T03:19:52</t>
+        </is>
+      </c>
+      <c r="T12" t="inlineStr">
+        <is>
+          <t>2014-03-18T03:19:53</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1382,6 +1622,26 @@
           <t>2014-03-18T07:27:21</t>
         </is>
       </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>2014-03-18T07:27:23</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>2014-03-18T07:27:23</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1454,6 +1714,26 @@
           <t>2014-03-18T13:52:09</t>
         </is>
       </c>
+      <c r="Q14" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R14" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="S14" t="inlineStr">
+        <is>
+          <t>2014-03-18T13:52:12</t>
+        </is>
+      </c>
+      <c r="T14" t="inlineStr">
+        <is>
+          <t>2014-03-18T13:52:12</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1526,6 +1806,26 @@
           <t>2014-03-18T16:08:31</t>
         </is>
       </c>
+      <c r="Q15" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R15" t="inlineStr">
+        <is>
+          <t>PATCX</t>
+        </is>
+      </c>
+      <c r="S15" t="inlineStr">
+        <is>
+          <t>2014-03-18T16:08:33</t>
+        </is>
+      </c>
+      <c r="T15" t="inlineStr">
+        <is>
+          <t>2014-03-18T16:08:34</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1598,6 +1898,26 @@
           <t>2014-03-18T17:32:13</t>
         </is>
       </c>
+      <c r="Q16" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R16" t="inlineStr">
+        <is>
+          <t>PX02</t>
+        </is>
+      </c>
+      <c r="S16" t="inlineStr">
+        <is>
+          <t>2014-03-18T17:32:15</t>
+        </is>
+      </c>
+      <c r="T16" t="inlineStr">
+        <is>
+          <t>2014-03-18T17:32:15</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1670,6 +1990,26 @@
           <t>2014-03-18T20:32:31</t>
         </is>
       </c>
+      <c r="Q17" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R17" t="inlineStr">
+        <is>
+          <t>PATCX</t>
+        </is>
+      </c>
+      <c r="S17" t="inlineStr">
+        <is>
+          <t>2014-03-18T20:32:32</t>
+        </is>
+      </c>
+      <c r="T17" t="inlineStr">
+        <is>
+          <t>2014-03-18T20:32:34</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1742,6 +2082,26 @@
           <t>2014-03-19T01:19:33</t>
         </is>
       </c>
+      <c r="Q18" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R18" t="inlineStr">
+        <is>
+          <t>PX02</t>
+        </is>
+      </c>
+      <c r="S18" t="inlineStr">
+        <is>
+          <t>2014-03-19T01:19:34</t>
+        </is>
+      </c>
+      <c r="T18" t="inlineStr">
+        <is>
+          <t>2014-03-19T01:19:35</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1814,6 +2174,26 @@
           <t>2014-03-19T12:42:36</t>
         </is>
       </c>
+      <c r="Q19" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R19" t="inlineStr">
+        <is>
+          <t>PX02</t>
+        </is>
+      </c>
+      <c r="S19" t="inlineStr">
+        <is>
+          <t>2014-03-19T12:42:37</t>
+        </is>
+      </c>
+      <c r="T19" t="inlineStr">
+        <is>
+          <t>2014-03-19T12:42:38</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1886,6 +2266,26 @@
           <t>2014-03-19T16:35:44</t>
         </is>
       </c>
+      <c r="Q20" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R20" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="S20" t="inlineStr">
+        <is>
+          <t>2014-03-19T16:35:46</t>
+        </is>
+      </c>
+      <c r="T20" t="inlineStr">
+        <is>
+          <t>2014-03-19T16:35:47</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1958,6 +2358,26 @@
           <t>2014-03-19T16:59:19</t>
         </is>
       </c>
+      <c r="Q21" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R21" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="S21" t="inlineStr">
+        <is>
+          <t>2014-03-19T16:59:21</t>
+        </is>
+      </c>
+      <c r="T21" t="inlineStr">
+        <is>
+          <t>2014-03-19T16:59:21</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -2030,6 +2450,26 @@
           <t>2014-03-21T18:29:34</t>
         </is>
       </c>
+      <c r="Q22" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R22" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>2014-03-21T18:29:35</t>
+        </is>
+      </c>
+      <c r="T22" t="inlineStr">
+        <is>
+          <t>2014-03-21T18:29:35</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -2102,6 +2542,26 @@
           <t>2014-03-24T00:42:17</t>
         </is>
       </c>
+      <c r="Q23" t="inlineStr">
+        <is>
+          <t>PATCX</t>
+        </is>
+      </c>
+      <c r="R23" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>2014-03-24T00:42:19</t>
+        </is>
+      </c>
+      <c r="T23" t="inlineStr">
+        <is>
+          <t>2014-03-24T00:42:19</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -2174,6 +2634,26 @@
           <t>2014-03-24T03:39:16</t>
         </is>
       </c>
+      <c r="Q24" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R24" t="inlineStr">
+        <is>
+          <t>PATCX</t>
+        </is>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>2014-03-24T03:39:17</t>
+        </is>
+      </c>
+      <c r="T24" t="inlineStr">
+        <is>
+          <t>2014-03-24T03:39:19</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -2246,6 +2726,26 @@
           <t>2014-03-24T04:41:56</t>
         </is>
       </c>
+      <c r="Q25" t="inlineStr">
+        <is>
+          <t>HMBCX</t>
+        </is>
+      </c>
+      <c r="R25" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>2014-03-24T04:41:56</t>
+        </is>
+      </c>
+      <c r="T25" t="inlineStr">
+        <is>
+          <t>2014-03-24T04:41:56</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -2318,6 +2818,26 @@
           <t>2014-03-25T12:39:33</t>
         </is>
       </c>
+      <c r="Q26" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R26" t="inlineStr">
+        <is>
+          <t>PX02</t>
+        </is>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>2014-03-25T12:39:35</t>
+        </is>
+      </c>
+      <c r="T26" t="inlineStr">
+        <is>
+          <t>2014-03-25T12:39:36</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -2390,6 +2910,26 @@
           <t>2014-03-25T19:08:04</t>
         </is>
       </c>
+      <c r="Q27" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R27" t="inlineStr">
+        <is>
+          <t>PB12</t>
+        </is>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>2014-03-25T19:08:04</t>
+        </is>
+      </c>
+      <c r="T27" t="inlineStr">
+        <is>
+          <t>2014-03-25T19:08:06</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -2462,6 +3002,26 @@
           <t>2014-03-26T07:07:45</t>
         </is>
       </c>
+      <c r="Q28" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R28" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>2014-03-26T07:07:46</t>
+        </is>
+      </c>
+      <c r="T28" t="inlineStr">
+        <is>
+          <t>2014-03-26T07:07:47</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2534,6 +3094,26 @@
           <t>2014-03-26T11:29:56</t>
         </is>
       </c>
+      <c r="Q29" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R29" t="inlineStr">
+        <is>
+          <t>PB12</t>
+        </is>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>2014-03-26T11:29:57</t>
+        </is>
+      </c>
+      <c r="T29" t="inlineStr">
+        <is>
+          <t>2014-03-26T11:29:57</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -2606,6 +3186,26 @@
           <t>2014-03-27T02:28:06</t>
         </is>
       </c>
+      <c r="Q30" t="inlineStr">
+        <is>
+          <t>TA01</t>
+        </is>
+      </c>
+      <c r="R30" t="inlineStr">
+        <is>
+          <t>PB12</t>
+        </is>
+      </c>
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>2014-03-27T02:28:07</t>
+        </is>
+      </c>
+      <c r="T30" t="inlineStr">
+        <is>
+          <t>2014-03-27T02:28:08</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -2678,6 +3278,26 @@
           <t>2014-03-27T02:32:35</t>
         </is>
       </c>
+      <c r="Q31" t="inlineStr">
+        <is>
+          <t>TA01</t>
+        </is>
+      </c>
+      <c r="R31" t="inlineStr">
+        <is>
+          <t>HMBCX</t>
+        </is>
+      </c>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>2014-03-27T02:32:36</t>
+        </is>
+      </c>
+      <c r="T31" t="inlineStr">
+        <is>
+          <t>2014-03-27T02:32:36</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -2750,6 +3370,26 @@
           <t>2014-03-27T07:32:26</t>
         </is>
       </c>
+      <c r="Q32" t="inlineStr">
+        <is>
+          <t>PSGCX</t>
+        </is>
+      </c>
+      <c r="R32" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>2014-03-27T07:32:26</t>
+        </is>
+      </c>
+      <c r="T32" t="inlineStr">
+        <is>
+          <t>2014-03-27T07:32:26</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -2822,6 +3462,26 @@
           <t>2014-03-27T09:31:19</t>
         </is>
       </c>
+      <c r="Q33" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R33" t="inlineStr">
+        <is>
+          <t>PX02</t>
+        </is>
+      </c>
+      <c r="S33" t="inlineStr">
+        <is>
+          <t>2014-03-27T09:31:19</t>
+        </is>
+      </c>
+      <c r="T33" t="inlineStr">
+        <is>
+          <t>2014-03-27T09:31:20</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2894,6 +3554,26 @@
           <t>2014-03-28T04:19:48</t>
         </is>
       </c>
+      <c r="Q34" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R34" t="inlineStr">
+        <is>
+          <t>PATCX</t>
+        </is>
+      </c>
+      <c r="S34" t="inlineStr">
+        <is>
+          <t>2014-03-28T04:19:49</t>
+        </is>
+      </c>
+      <c r="T34" t="inlineStr">
+        <is>
+          <t>2014-03-28T04:19:51</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -2966,6 +3646,26 @@
           <t>2014-03-28T05:55:54</t>
         </is>
       </c>
+      <c r="Q35" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R35" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="S35" t="inlineStr">
+        <is>
+          <t>2014-03-28T05:55:57</t>
+        </is>
+      </c>
+      <c r="T35" t="inlineStr">
+        <is>
+          <t>2014-03-28T05:55:57</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -3038,6 +3738,26 @@
           <t>2014-03-29T06:57:14</t>
         </is>
       </c>
+      <c r="Q36" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R36" t="inlineStr">
+        <is>
+          <t>PX02</t>
+        </is>
+      </c>
+      <c r="S36" t="inlineStr">
+        <is>
+          <t>2014-03-29T06:57:15</t>
+        </is>
+      </c>
+      <c r="T36" t="inlineStr">
+        <is>
+          <t>2014-03-29T06:57:15</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -3110,6 +3830,26 @@
           <t>2017-04-24T07:15:46</t>
         </is>
       </c>
+      <c r="Q37" t="inlineStr">
+        <is>
+          <t>ROC1</t>
+        </is>
+      </c>
+      <c r="R37" t="inlineStr">
+        <is>
+          <t>MT07</t>
+        </is>
+      </c>
+      <c r="S37" t="inlineStr">
+        <is>
+          <t>2017-04-24T07:15:47</t>
+        </is>
+      </c>
+      <c r="T37" t="inlineStr">
+        <is>
+          <t>2017-04-24T07:15:47</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -3182,6 +3922,26 @@
           <t>2014-04-01T01:06:54</t>
         </is>
       </c>
+      <c r="Q38" t="inlineStr">
+        <is>
+          <t>HMBCX</t>
+        </is>
+      </c>
+      <c r="R38" t="inlineStr">
+        <is>
+          <t>AP01</t>
+        </is>
+      </c>
+      <c r="S38" t="inlineStr">
+        <is>
+          <t>2014-04-01T01:06:55</t>
+        </is>
+      </c>
+      <c r="T38" t="inlineStr">
+        <is>
+          <t>2014-04-01T01:06:56</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -3254,6 +4014,26 @@
           <t>2014-04-02T15:37:16</t>
         </is>
       </c>
+      <c r="Q39" t="inlineStr">
+        <is>
+          <t>PX02</t>
+        </is>
+      </c>
+      <c r="R39" t="inlineStr">
+        <is>
+          <t>PATCX</t>
+        </is>
+      </c>
+      <c r="S39" t="inlineStr">
+        <is>
+          <t>2014-04-02T15:37:16</t>
+        </is>
+      </c>
+      <c r="T39" t="inlineStr">
+        <is>
+          <t>2014-04-02T15:37:18</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -3326,6 +4106,26 @@
           <t>2014-04-04T11:29:20</t>
         </is>
       </c>
+      <c r="Q40" t="inlineStr">
+        <is>
+          <t>AP01</t>
+        </is>
+      </c>
+      <c r="R40" t="inlineStr">
+        <is>
+          <t>TA02</t>
+        </is>
+      </c>
+      <c r="S40" t="inlineStr">
+        <is>
+          <t>2014-04-04T11:29:21</t>
+        </is>
+      </c>
+      <c r="T40" t="inlineStr">
+        <is>
+          <t>2014-04-04T11:29:21</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -3398,6 +4198,26 @@
           <t>2014-04-04T21:53:46</t>
         </is>
       </c>
+      <c r="Q41" t="inlineStr">
+        <is>
+          <t>HMBCX</t>
+        </is>
+      </c>
+      <c r="R41" t="inlineStr">
+        <is>
+          <t>PB12</t>
+        </is>
+      </c>
+      <c r="S41" t="inlineStr">
+        <is>
+          <t>2014-04-04T21:53:46</t>
+        </is>
+      </c>
+      <c r="T41" t="inlineStr">
+        <is>
+          <t>2014-04-04T21:53:46</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -3470,6 +4290,26 @@
           <t>2014-04-06T05:14:24</t>
         </is>
       </c>
+      <c r="Q42" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="R42" t="inlineStr">
+        <is>
+          <t>PSGCX</t>
+        </is>
+      </c>
+      <c r="S42" t="inlineStr">
+        <is>
+          <t>2014-04-06T05:14:24</t>
+        </is>
+      </c>
+      <c r="T42" t="inlineStr">
+        <is>
+          <t>2014-04-06T05:14:25</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -3542,6 +4382,26 @@
           <t>2014-04-07T09:54:42</t>
         </is>
       </c>
+      <c r="Q43" t="inlineStr">
+        <is>
+          <t>PSGCX</t>
+        </is>
+      </c>
+      <c r="R43" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="S43" t="inlineStr">
+        <is>
+          <t>2014-04-07T09:54:43</t>
+        </is>
+      </c>
+      <c r="T43" t="inlineStr">
+        <is>
+          <t>2014-04-07T09:54:43</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -3614,6 +4474,26 @@
           <t>2014-04-09T00:42:02</t>
         </is>
       </c>
+      <c r="Q44" t="inlineStr">
+        <is>
+          <t>MNMCX</t>
+        </is>
+      </c>
+      <c r="R44" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="S44" t="inlineStr">
+        <is>
+          <t>2014-04-09T00:42:02</t>
+        </is>
+      </c>
+      <c r="T44" t="inlineStr">
+        <is>
+          <t>2014-04-09T00:42:02</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -3686,6 +4566,26 @@
           <t>2014-04-10T09:14:25</t>
         </is>
       </c>
+      <c r="Q45" t="inlineStr">
+        <is>
+          <t>PSGCX</t>
+        </is>
+      </c>
+      <c r="R45" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="S45" t="inlineStr">
+        <is>
+          <t>2014-04-10T09:14:25</t>
+        </is>
+      </c>
+      <c r="T45" t="inlineStr">
+        <is>
+          <t>2014-04-10T09:14:25</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -3758,6 +4658,26 @@
           <t>2014-04-10T15:47:31</t>
         </is>
       </c>
+      <c r="Q46" t="inlineStr">
+        <is>
+          <t>PATCX</t>
+        </is>
+      </c>
+      <c r="R46" t="inlineStr">
+        <is>
+          <t>PB01</t>
+        </is>
+      </c>
+      <c r="S46" t="inlineStr">
+        <is>
+          <t>2014-04-10T15:47:32</t>
+        </is>
+      </c>
+      <c r="T46" t="inlineStr">
+        <is>
+          <t>2014-04-10T15:47:32</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -3830,6 +4750,26 @@
           <t>2014-04-12T17:17:02</t>
         </is>
       </c>
+      <c r="Q47" t="inlineStr">
+        <is>
+          <t>PX05</t>
+        </is>
+      </c>
+      <c r="R47" t="inlineStr">
+        <is>
+          <t>PB07</t>
+        </is>
+      </c>
+      <c r="S47" t="inlineStr">
+        <is>
+          <t>2014-04-12T17:17:03</t>
+        </is>
+      </c>
+      <c r="T47" t="inlineStr">
+        <is>
+          <t>2014-04-12T17:17:05</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -3902,6 +4842,26 @@
           <t>2014-04-19T12:57:30</t>
         </is>
       </c>
+      <c r="Q48" t="inlineStr">
+        <is>
+          <t>PX02</t>
+        </is>
+      </c>
+      <c r="R48" t="inlineStr">
+        <is>
+          <t>PATCX</t>
+        </is>
+      </c>
+      <c r="S48" t="inlineStr">
+        <is>
+          <t>2014-04-19T12:57:30</t>
+        </is>
+      </c>
+      <c r="T48" t="inlineStr">
+        <is>
+          <t>2014-04-19T12:57:31</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -3974,6 +4934,26 @@
           <t>2014-04-19T18:22:04</t>
         </is>
       </c>
+      <c r="Q49" t="inlineStr">
+        <is>
+          <t>PB05</t>
+        </is>
+      </c>
+      <c r="R49" t="inlineStr">
+        <is>
+          <t>PB06</t>
+        </is>
+      </c>
+      <c r="S49" t="inlineStr">
+        <is>
+          <t>2014-04-19T18:22:05</t>
+        </is>
+      </c>
+      <c r="T49" t="inlineStr">
+        <is>
+          <t>2014-04-19T18:22:07</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -4046,6 +5026,26 @@
           <t>2014-04-19T18:39:57</t>
         </is>
       </c>
+      <c r="Q50" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R50" t="inlineStr">
+        <is>
+          <t>PB01</t>
+        </is>
+      </c>
+      <c r="S50" t="inlineStr">
+        <is>
+          <t>2014-04-19T18:40:00</t>
+        </is>
+      </c>
+      <c r="T50" t="inlineStr">
+        <is>
+          <t>2014-04-19T18:40:01</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -4118,6 +5118,26 @@
           <t>2014-04-22T02:14:38</t>
         </is>
       </c>
+      <c r="Q51" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="R51" t="inlineStr">
+        <is>
+          <t>PB01</t>
+        </is>
+      </c>
+      <c r="S51" t="inlineStr">
+        <is>
+          <t>2014-04-22T02:14:40</t>
+        </is>
+      </c>
+      <c r="T51" t="inlineStr">
+        <is>
+          <t>2014-04-22T02:14:42</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -4190,6 +5210,26 @@
           <t>2014-04-23T11:42:07</t>
         </is>
       </c>
+      <c r="Q52" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R52" t="inlineStr">
+        <is>
+          <t>PB01</t>
+        </is>
+      </c>
+      <c r="S52" t="inlineStr">
+        <is>
+          <t>2014-04-23T11:42:08</t>
+        </is>
+      </c>
+      <c r="T52" t="inlineStr">
+        <is>
+          <t>2014-04-23T11:42:10</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -4262,6 +5302,26 @@
           <t>2014-04-24T20:28:48</t>
         </is>
       </c>
+      <c r="Q53" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="R53" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="S53" t="inlineStr">
+        <is>
+          <t>2014-04-24T20:28:50</t>
+        </is>
+      </c>
+      <c r="T53" t="inlineStr">
+        <is>
+          <t>2014-04-24T20:28:51</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -4334,6 +5394,26 @@
           <t>2014-04-27T03:16:01</t>
         </is>
       </c>
+      <c r="Q54" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R54" t="inlineStr">
+        <is>
+          <t>PX02</t>
+        </is>
+      </c>
+      <c r="S54" t="inlineStr">
+        <is>
+          <t>2014-04-27T03:16:03</t>
+        </is>
+      </c>
+      <c r="T54" t="inlineStr">
+        <is>
+          <t>2014-04-27T03:16:03</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -4406,6 +5486,26 @@
           <t>2014-04-30T12:48:26</t>
         </is>
       </c>
+      <c r="Q55" t="inlineStr">
+        <is>
+          <t>PB06</t>
+        </is>
+      </c>
+      <c r="R55" t="inlineStr">
+        <is>
+          <t>PB02</t>
+        </is>
+      </c>
+      <c r="S55" t="inlineStr">
+        <is>
+          <t>2014-04-30T12:48:26</t>
+        </is>
+      </c>
+      <c r="T55" t="inlineStr">
+        <is>
+          <t>2014-04-30T12:48:29</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -4478,6 +5578,26 @@
           <t>2014-05-01T09:39:53</t>
         </is>
       </c>
+      <c r="Q56" t="inlineStr">
+        <is>
+          <t>PX05</t>
+        </is>
+      </c>
+      <c r="R56" t="inlineStr">
+        <is>
+          <t>PB03</t>
+        </is>
+      </c>
+      <c r="S56" t="inlineStr">
+        <is>
+          <t>2014-05-01T09:39:53</t>
+        </is>
+      </c>
+      <c r="T56" t="inlineStr">
+        <is>
+          <t>2014-05-01T09:39:54</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -4550,6 +5670,26 @@
           <t>2014-05-02T08:28:45</t>
         </is>
       </c>
+      <c r="Q57" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R57" t="inlineStr">
+        <is>
+          <t>PATCX</t>
+        </is>
+      </c>
+      <c r="S57" t="inlineStr">
+        <is>
+          <t>2014-05-02T08:28:46</t>
+        </is>
+      </c>
+      <c r="T57" t="inlineStr">
+        <is>
+          <t>2014-05-02T08:28:47</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -4622,6 +5762,26 @@
           <t>2014-05-03T15:55:30</t>
         </is>
       </c>
+      <c r="Q58" t="inlineStr">
+        <is>
+          <t>AP01</t>
+        </is>
+      </c>
+      <c r="R58" t="inlineStr">
+        <is>
+          <t>TA02</t>
+        </is>
+      </c>
+      <c r="S58" t="inlineStr">
+        <is>
+          <t>2014-05-03T15:55:31</t>
+        </is>
+      </c>
+      <c r="T58" t="inlineStr">
+        <is>
+          <t>2014-05-03T15:55:32</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -4694,6 +5854,26 @@
           <t>2014-05-03T19:25:06</t>
         </is>
       </c>
+      <c r="Q59" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R59" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="S59" t="inlineStr">
+        <is>
+          <t>2014-05-03T19:25:07</t>
+        </is>
+      </c>
+      <c r="T59" t="inlineStr">
+        <is>
+          <t>2014-05-03T19:25:08</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -4766,6 +5946,26 @@
           <t>2014-05-06T15:04:06</t>
         </is>
       </c>
+      <c r="Q60" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="R60" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="S60" t="inlineStr">
+        <is>
+          <t>2014-05-06T15:04:06</t>
+        </is>
+      </c>
+      <c r="T60" t="inlineStr">
+        <is>
+          <t>2014-05-06T15:04:08</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -4838,6 +6038,26 @@
           <t>2014-05-11T00:35:59</t>
         </is>
       </c>
+      <c r="Q61" t="inlineStr">
+        <is>
+          <t>PB01</t>
+        </is>
+      </c>
+      <c r="R61" t="inlineStr">
+        <is>
+          <t>PB02</t>
+        </is>
+      </c>
+      <c r="S61" t="inlineStr">
+        <is>
+          <t>2014-05-11T00:36:03</t>
+        </is>
+      </c>
+      <c r="T61" t="inlineStr">
+        <is>
+          <t>2014-05-11T00:36:04</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -4910,6 +6130,26 @@
           <t>2014-05-12T09:10:41</t>
         </is>
       </c>
+      <c r="Q62" t="inlineStr">
+        <is>
+          <t>PB16</t>
+        </is>
+      </c>
+      <c r="R62" t="inlineStr">
+        <is>
+          <t>MNMCX</t>
+        </is>
+      </c>
+      <c r="S62" t="inlineStr">
+        <is>
+          <t>2014-05-12T09:10:41</t>
+        </is>
+      </c>
+      <c r="T62" t="inlineStr">
+        <is>
+          <t>2014-05-12T09:10:42</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -4982,6 +6222,26 @@
           <t>2014-05-15T06:10:47</t>
         </is>
       </c>
+      <c r="Q63" t="inlineStr">
+        <is>
+          <t>V25A</t>
+        </is>
+      </c>
+      <c r="R63" t="inlineStr">
+        <is>
+          <t>CO02</t>
+        </is>
+      </c>
+      <c r="S63" t="inlineStr">
+        <is>
+          <t>2014-05-15T06:10:48</t>
+        </is>
+      </c>
+      <c r="T63" t="inlineStr">
+        <is>
+          <t>2014-05-15T06:10:49</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -5054,6 +6314,26 @@
           <t>2014-05-16T05:44:57</t>
         </is>
       </c>
+      <c r="Q64" t="inlineStr">
+        <is>
+          <t>GO01</t>
+        </is>
+      </c>
+      <c r="R64" t="inlineStr">
+        <is>
+          <t>PB08</t>
+        </is>
+      </c>
+      <c r="S64" t="inlineStr">
+        <is>
+          <t>2014-05-16T05:44:59</t>
+        </is>
+      </c>
+      <c r="T64" t="inlineStr">
+        <is>
+          <t>2014-05-16T05:44:59</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -5126,6 +6406,26 @@
           <t>2014-05-20T09:19:17</t>
         </is>
       </c>
+      <c r="Q65" t="inlineStr">
+        <is>
+          <t>PB12</t>
+        </is>
+      </c>
+      <c r="R65" t="inlineStr">
+        <is>
+          <t>HMBCX</t>
+        </is>
+      </c>
+      <c r="S65" t="inlineStr">
+        <is>
+          <t>2014-05-20T09:19:17</t>
+        </is>
+      </c>
+      <c r="T65" t="inlineStr">
+        <is>
+          <t>2014-05-20T09:19:18</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -5198,6 +6498,26 @@
           <t>2014-05-20T10:46:51</t>
         </is>
       </c>
+      <c r="Q66" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="R66" t="inlineStr">
+        <is>
+          <t>PB07</t>
+        </is>
+      </c>
+      <c r="S66" t="inlineStr">
+        <is>
+          <t>2014-05-20T10:46:53</t>
+        </is>
+      </c>
+      <c r="T66" t="inlineStr">
+        <is>
+          <t>2014-05-20T10:46:54</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -5270,6 +6590,26 @@
           <t>2014-05-21T15:01:12</t>
         </is>
       </c>
+      <c r="Q67" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R67" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="S67" t="inlineStr">
+        <is>
+          <t>2014-05-21T15:01:14</t>
+        </is>
+      </c>
+      <c r="T67" t="inlineStr">
+        <is>
+          <t>2014-05-21T15:01:14</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -5342,6 +6682,26 @@
           <t>2014-05-23T01:27:18</t>
         </is>
       </c>
+      <c r="Q68" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R68" t="inlineStr">
+        <is>
+          <t>PB12</t>
+        </is>
+      </c>
+      <c r="S68" t="inlineStr">
+        <is>
+          <t>2014-05-23T01:27:19</t>
+        </is>
+      </c>
+      <c r="T68" t="inlineStr">
+        <is>
+          <t>2014-05-23T01:27:20</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -5414,6 +6774,26 @@
           <t>2014-05-24T22:18:06</t>
         </is>
       </c>
+      <c r="Q69" t="inlineStr">
+        <is>
+          <t>MNMCX</t>
+        </is>
+      </c>
+      <c r="R69" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="S69" t="inlineStr">
+        <is>
+          <t>2014-05-24T22:18:07</t>
+        </is>
+      </c>
+      <c r="T69" t="inlineStr">
+        <is>
+          <t>2014-05-24T22:18:07</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -5486,6 +6866,26 @@
           <t>2014-05-27T20:54:36</t>
         </is>
       </c>
+      <c r="Q70" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="R70" t="inlineStr">
+        <is>
+          <t>PX02</t>
+        </is>
+      </c>
+      <c r="S70" t="inlineStr">
+        <is>
+          <t>2014-05-27T20:54:38</t>
+        </is>
+      </c>
+      <c r="T70" t="inlineStr">
+        <is>
+          <t>2014-05-27T20:54:39</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -5558,6 +6958,26 @@
           <t>2014-05-31T18:57:34</t>
         </is>
       </c>
+      <c r="Q71" t="inlineStr">
+        <is>
+          <t>MNMCX</t>
+        </is>
+      </c>
+      <c r="R71" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="S71" t="inlineStr">
+        <is>
+          <t>2014-05-31T18:57:35</t>
+        </is>
+      </c>
+      <c r="T71" t="inlineStr">
+        <is>
+          <t>2014-05-31T18:57:35</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -5630,6 +7050,26 @@
           <t>2014-06-01T12:13:18</t>
         </is>
       </c>
+      <c r="Q72" t="inlineStr">
+        <is>
+          <t>PATCX</t>
+        </is>
+      </c>
+      <c r="R72" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="S72" t="inlineStr">
+        <is>
+          <t>2014-06-01T12:13:19</t>
+        </is>
+      </c>
+      <c r="T72" t="inlineStr">
+        <is>
+          <t>2014-06-01T12:13:19</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -5702,6 +7142,26 @@
           <t>2014-06-04T17:27:53</t>
         </is>
       </c>
+      <c r="Q73" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="R73" t="inlineStr">
+        <is>
+          <t>PB01</t>
+        </is>
+      </c>
+      <c r="S73" t="inlineStr">
+        <is>
+          <t>2014-06-04T17:27:54</t>
+        </is>
+      </c>
+      <c r="T73" t="inlineStr">
+        <is>
+          <t>2014-06-04T17:27:56</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -5774,6 +7234,26 @@
           <t>2014-06-20T15:43:28</t>
         </is>
       </c>
+      <c r="Q74" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="R74" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="S74" t="inlineStr">
+        <is>
+          <t>2014-06-20T15:43:28</t>
+        </is>
+      </c>
+      <c r="T74" t="inlineStr">
+        <is>
+          <t>2014-06-20T15:43:30</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -5846,6 +7326,26 @@
           <t>2014-06-20T18:05:43</t>
         </is>
       </c>
+      <c r="Q75" t="inlineStr">
+        <is>
+          <t>PX05</t>
+        </is>
+      </c>
+      <c r="R75" t="inlineStr">
+        <is>
+          <t>PB07</t>
+        </is>
+      </c>
+      <c r="S75" t="inlineStr">
+        <is>
+          <t>2014-06-20T18:05:43</t>
+        </is>
+      </c>
+      <c r="T75" t="inlineStr">
+        <is>
+          <t>2014-06-20T18:05:46</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -5918,6 +7418,26 @@
           <t>2014-06-21T07:22:47</t>
         </is>
       </c>
+      <c r="Q76" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="R76" t="inlineStr">
+        <is>
+          <t>PB01</t>
+        </is>
+      </c>
+      <c r="S76" t="inlineStr">
+        <is>
+          <t>2014-06-21T07:22:49</t>
+        </is>
+      </c>
+      <c r="T76" t="inlineStr">
+        <is>
+          <t>2014-06-21T07:22:50</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -5990,6 +7510,26 @@
           <t>2014-07-04T19:58:22</t>
         </is>
       </c>
+      <c r="Q77" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="R77" t="inlineStr">
+        <is>
+          <t>PB02</t>
+        </is>
+      </c>
+      <c r="S77" t="inlineStr">
+        <is>
+          <t>2014-07-04T19:58:22</t>
+        </is>
+      </c>
+      <c r="T77" t="inlineStr">
+        <is>
+          <t>2014-07-04T19:58:23</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -6062,6 +7602,26 @@
           <t>2014-07-08T17:19:53</t>
         </is>
       </c>
+      <c r="Q78" t="inlineStr">
+        <is>
+          <t>PSGCX</t>
+        </is>
+      </c>
+      <c r="R78" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="S78" t="inlineStr">
+        <is>
+          <t>2014-07-08T17:19:54</t>
+        </is>
+      </c>
+      <c r="T78" t="inlineStr">
+        <is>
+          <t>2014-07-08T17:19:56</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -6134,6 +7694,26 @@
           <t>2014-07-08T20:42:36</t>
         </is>
       </c>
+      <c r="Q79" t="inlineStr">
+        <is>
+          <t>PSGCX</t>
+        </is>
+      </c>
+      <c r="R79" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="S79" t="inlineStr">
+        <is>
+          <t>2014-07-08T20:42:37</t>
+        </is>
+      </c>
+      <c r="T79" t="inlineStr">
+        <is>
+          <t>2014-07-08T20:42:39</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -6206,6 +7786,26 @@
           <t>2014-07-11T10:37:43</t>
         </is>
       </c>
+      <c r="Q80" t="inlineStr">
+        <is>
+          <t>PX05</t>
+        </is>
+      </c>
+      <c r="R80" t="inlineStr">
+        <is>
+          <t>PB20</t>
+        </is>
+      </c>
+      <c r="S80" t="inlineStr">
+        <is>
+          <t>2014-07-11T10:37:44</t>
+        </is>
+      </c>
+      <c r="T80" t="inlineStr">
+        <is>
+          <t>2014-07-11T10:37:46</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -6278,6 +7878,26 @@
           <t>2014-07-12T01:54:05</t>
         </is>
       </c>
+      <c r="Q81" t="inlineStr">
+        <is>
+          <t>IN40</t>
+        </is>
+      </c>
+      <c r="R81" t="inlineStr">
+        <is>
+          <t>IN41</t>
+        </is>
+      </c>
+      <c r="S81" t="inlineStr">
+        <is>
+          <t>2014-07-12T01:54:06</t>
+        </is>
+      </c>
+      <c r="T81" t="inlineStr">
+        <is>
+          <t>2014-07-12T01:54:06</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -6350,6 +7970,26 @@
           <t>2014-07-12T11:45:14</t>
         </is>
       </c>
+      <c r="Q82" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="R82" t="inlineStr">
+        <is>
+          <t>PB01</t>
+        </is>
+      </c>
+      <c r="S82" t="inlineStr">
+        <is>
+          <t>2014-07-12T11:45:17</t>
+        </is>
+      </c>
+      <c r="T82" t="inlineStr">
+        <is>
+          <t>2014-07-12T11:45:18</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -6422,6 +8062,26 @@
           <t>2014-07-13T13:13:25</t>
         </is>
       </c>
+      <c r="Q83" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="R83" t="inlineStr">
+        <is>
+          <t>HMBCX</t>
+        </is>
+      </c>
+      <c r="S83" t="inlineStr">
+        <is>
+          <t>2014-07-13T13:13:26</t>
+        </is>
+      </c>
+      <c r="T83" t="inlineStr">
+        <is>
+          <t>2014-07-13T13:13:27</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -6494,6 +8154,26 @@
           <t>2014-07-22T04:27:54</t>
         </is>
       </c>
+      <c r="Q84" t="inlineStr">
+        <is>
+          <t>PB06</t>
+        </is>
+      </c>
+      <c r="R84" t="inlineStr">
+        <is>
+          <t>PB02</t>
+        </is>
+      </c>
+      <c r="S84" t="inlineStr">
+        <is>
+          <t>2014-07-22T04:27:55</t>
+        </is>
+      </c>
+      <c r="T84" t="inlineStr">
+        <is>
+          <t>2014-07-22T04:27:56</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -6566,6 +8246,26 @@
           <t>2014-07-29T15:28:24</t>
         </is>
       </c>
+      <c r="Q85" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="R85" t="inlineStr">
+        <is>
+          <t>PB01</t>
+        </is>
+      </c>
+      <c r="S85" t="inlineStr">
+        <is>
+          <t>2014-07-29T15:28:25</t>
+        </is>
+      </c>
+      <c r="T85" t="inlineStr">
+        <is>
+          <t>2014-07-29T15:28:27</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -6638,6 +8338,26 @@
           <t>2014-08-04T13:07:22</t>
         </is>
       </c>
+      <c r="Q86" t="inlineStr">
+        <is>
+          <t>PB08</t>
+        </is>
+      </c>
+      <c r="R86" t="inlineStr">
+        <is>
+          <t>PATCX</t>
+        </is>
+      </c>
+      <c r="S86" t="inlineStr">
+        <is>
+          <t>2014-08-04T13:07:24</t>
+        </is>
+      </c>
+      <c r="T86" t="inlineStr">
+        <is>
+          <t>2014-08-04T13:07:25</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -6710,6 +8430,26 @@
           <t>2014-08-10T20:42:26</t>
         </is>
       </c>
+      <c r="Q87" t="inlineStr">
+        <is>
+          <t>TA02</t>
+        </is>
+      </c>
+      <c r="R87" t="inlineStr">
+        <is>
+          <t>PB08</t>
+        </is>
+      </c>
+      <c r="S87" t="inlineStr">
+        <is>
+          <t>2014-08-10T20:42:27</t>
+        </is>
+      </c>
+      <c r="T87" t="inlineStr">
+        <is>
+          <t>2014-08-10T20:42:27</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -6782,6 +8522,26 @@
           <t>2014-08-27T21:10:13</t>
         </is>
       </c>
+      <c r="Q88" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R88" t="inlineStr">
+        <is>
+          <t>PB12</t>
+        </is>
+      </c>
+      <c r="S88" t="inlineStr">
+        <is>
+          <t>2014-08-27T21:10:13</t>
+        </is>
+      </c>
+      <c r="T88" t="inlineStr">
+        <is>
+          <t>2014-08-27T21:10:15</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -6854,6 +8614,26 @@
           <t>2014-09-23T03:43:55</t>
         </is>
       </c>
+      <c r="Q89" t="inlineStr">
+        <is>
+          <t>PATCX</t>
+        </is>
+      </c>
+      <c r="R89" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="S89" t="inlineStr">
+        <is>
+          <t>2014-09-23T03:43:57</t>
+        </is>
+      </c>
+      <c r="T89" t="inlineStr">
+        <is>
+          <t>2014-09-23T03:43:57</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -6926,6 +8706,26 @@
           <t>2014-10-05T01:14:36</t>
         </is>
       </c>
+      <c r="Q90" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="R90" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="S90" t="inlineStr">
+        <is>
+          <t>2014-10-05T01:14:38</t>
+        </is>
+      </c>
+      <c r="T90" t="inlineStr">
+        <is>
+          <t>2014-10-05T01:14:39</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -6998,6 +8798,26 @@
           <t>2014-10-16T21:56:44</t>
         </is>
       </c>
+      <c r="Q91" t="inlineStr">
+        <is>
+          <t>PSGCX</t>
+        </is>
+      </c>
+      <c r="R91" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="S91" t="inlineStr">
+        <is>
+          <t>2014-10-16T21:56:46</t>
+        </is>
+      </c>
+      <c r="T91" t="inlineStr">
+        <is>
+          <t>2014-10-16T21:56:46</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -7070,6 +8890,26 @@
           <t>2014-12-10T02:38:11</t>
         </is>
       </c>
+      <c r="Q92" t="inlineStr">
+        <is>
+          <t>VA01</t>
+        </is>
+      </c>
+      <c r="R92" t="inlineStr">
+        <is>
+          <t>ROC1</t>
+        </is>
+      </c>
+      <c r="S92" t="inlineStr">
+        <is>
+          <t>2014-12-10T02:38:15</t>
+        </is>
+      </c>
+      <c r="T92" t="inlineStr">
+        <is>
+          <t>2014-12-10T02:38:16</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -7142,6 +8982,26 @@
           <t>2014-12-15T19:59:03</t>
         </is>
       </c>
+      <c r="Q93" t="inlineStr">
+        <is>
+          <t>MT02</t>
+        </is>
+      </c>
+      <c r="R93" t="inlineStr">
+        <is>
+          <t>VA01</t>
+        </is>
+      </c>
+      <c r="S93" t="inlineStr">
+        <is>
+          <t>2014-12-15T19:59:03</t>
+        </is>
+      </c>
+      <c r="T93" t="inlineStr">
+        <is>
+          <t>2014-12-15T19:59:03</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -7214,6 +9074,26 @@
           <t>2014-12-16T18:50:28</t>
         </is>
       </c>
+      <c r="Q94" t="inlineStr">
+        <is>
+          <t>IN41</t>
+        </is>
+      </c>
+      <c r="R94" t="inlineStr">
+        <is>
+          <t>GO04</t>
+        </is>
+      </c>
+      <c r="S94" t="inlineStr">
+        <is>
+          <t>2014-12-16T18:50:28</t>
+        </is>
+      </c>
+      <c r="T94" t="inlineStr">
+        <is>
+          <t>2014-12-16T18:50:32</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -7286,6 +9166,26 @@
           <t>2014-12-25T20:45:07</t>
         </is>
       </c>
+      <c r="Q95" t="inlineStr">
+        <is>
+          <t>PB15</t>
+        </is>
+      </c>
+      <c r="R95" t="inlineStr">
+        <is>
+          <t>PB05</t>
+        </is>
+      </c>
+      <c r="S95" t="inlineStr">
+        <is>
+          <t>2014-12-25T20:45:11</t>
+        </is>
+      </c>
+      <c r="T95" t="inlineStr">
+        <is>
+          <t>2014-12-25T20:45:14</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -7358,6 +9258,26 @@
           <t>2014-11-17T19:59:36</t>
         </is>
       </c>
+      <c r="Q96" t="inlineStr">
+        <is>
+          <t>ROC1</t>
+        </is>
+      </c>
+      <c r="R96" t="inlineStr">
+        <is>
+          <t>MT07</t>
+        </is>
+      </c>
+      <c r="S96" t="inlineStr">
+        <is>
+          <t>2014-11-17T19:59:37</t>
+        </is>
+      </c>
+      <c r="T96" t="inlineStr">
+        <is>
+          <t>2014-11-17T19:59:37</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -7430,6 +9350,26 @@
           <t>2014-11-19T11:21:49</t>
         </is>
       </c>
+      <c r="Q97" t="inlineStr">
+        <is>
+          <t>PB06</t>
+        </is>
+      </c>
+      <c r="R97" t="inlineStr">
+        <is>
+          <t>PB02</t>
+        </is>
+      </c>
+      <c r="S97" t="inlineStr">
+        <is>
+          <t>2014-11-19T11:21:52</t>
+        </is>
+      </c>
+      <c r="T97" t="inlineStr">
+        <is>
+          <t>2014-11-19T11:21:53</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -7502,6 +9442,26 @@
           <t>2014-11-23T08:54:39</t>
         </is>
       </c>
+      <c r="Q98" t="inlineStr">
+        <is>
+          <t>PB10</t>
+        </is>
+      </c>
+      <c r="R98" t="inlineStr">
+        <is>
+          <t>PX06</t>
+        </is>
+      </c>
+      <c r="S98" t="inlineStr">
+        <is>
+          <t>2014-11-23T08:54:39</t>
+        </is>
+      </c>
+      <c r="T98" t="inlineStr">
+        <is>
+          <t>2014-11-23T08:54:39</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -7574,6 +9534,26 @@
           <t>2014-11-27T11:15:37</t>
         </is>
       </c>
+      <c r="Q99" t="inlineStr">
+        <is>
+          <t>MT02</t>
+        </is>
+      </c>
+      <c r="R99" t="inlineStr">
+        <is>
+          <t>CO04</t>
+        </is>
+      </c>
+      <c r="S99" t="inlineStr">
+        <is>
+          <t>2014-11-27T11:15:38</t>
+        </is>
+      </c>
+      <c r="T99" t="inlineStr">
+        <is>
+          <t>2014-11-27T11:15:41</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -7646,6 +9626,26 @@
           <t>2015-01-02T12:08:48</t>
         </is>
       </c>
+      <c r="Q100" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R100" t="inlineStr">
+        <is>
+          <t>PSGCX</t>
+        </is>
+      </c>
+      <c r="S100" t="inlineStr">
+        <is>
+          <t>2015-01-02T12:08:51</t>
+        </is>
+      </c>
+      <c r="T100" t="inlineStr">
+        <is>
+          <t>2015-01-02T12:08:52</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
@@ -7718,6 +9718,26 @@
           <t>2015-01-07T17:19:18</t>
         </is>
       </c>
+      <c r="Q101" t="inlineStr">
+        <is>
+          <t>MNMCX</t>
+        </is>
+      </c>
+      <c r="R101" t="inlineStr">
+        <is>
+          <t>HMBCX</t>
+        </is>
+      </c>
+      <c r="S101" t="inlineStr">
+        <is>
+          <t>2015-01-07T17:19:19</t>
+        </is>
+      </c>
+      <c r="T101" t="inlineStr">
+        <is>
+          <t>2015-01-07T17:19:20</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
@@ -7790,6 +9810,26 @@
           <t>2015-01-18T19:32:40</t>
         </is>
       </c>
+      <c r="Q102" t="inlineStr">
+        <is>
+          <t>PB15</t>
+        </is>
+      </c>
+      <c r="R102" t="inlineStr">
+        <is>
+          <t>PB03</t>
+        </is>
+      </c>
+      <c r="S102" t="inlineStr">
+        <is>
+          <t>2015-01-18T19:32:41</t>
+        </is>
+      </c>
+      <c r="T102" t="inlineStr">
+        <is>
+          <t>2015-01-18T19:32:45</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
@@ -7862,6 +9902,26 @@
           <t>2015-01-26T01:38:39</t>
         </is>
       </c>
+      <c r="Q103" t="inlineStr">
+        <is>
+          <t>TLL</t>
+        </is>
+      </c>
+      <c r="R103" t="inlineStr">
+        <is>
+          <t>IN40</t>
+        </is>
+      </c>
+      <c r="S103" t="inlineStr">
+        <is>
+          <t>2015-01-26T01:38:39</t>
+        </is>
+      </c>
+      <c r="T103" t="inlineStr">
+        <is>
+          <t>2015-01-26T01:38:39</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
@@ -7934,6 +9994,26 @@
           <t>2015-01-27T09:59:58</t>
         </is>
       </c>
+      <c r="Q104" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="R104" t="inlineStr">
+        <is>
+          <t>PX02</t>
+        </is>
+      </c>
+      <c r="S104" t="inlineStr">
+        <is>
+          <t>2015-01-27T10:00:00</t>
+        </is>
+      </c>
+      <c r="T104" t="inlineStr">
+        <is>
+          <t>2015-01-27T10:00:01</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
@@ -8006,6 +10086,26 @@
           <t>2015-01-29T06:17:17</t>
         </is>
       </c>
+      <c r="Q105" t="inlineStr">
+        <is>
+          <t>V25A</t>
+        </is>
+      </c>
+      <c r="R105" t="inlineStr">
+        <is>
+          <t>VA03</t>
+        </is>
+      </c>
+      <c r="S105" t="inlineStr">
+        <is>
+          <t>2015-01-29T06:17:17</t>
+        </is>
+      </c>
+      <c r="T105" t="inlineStr">
+        <is>
+          <t>2015-01-29T06:17:19</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
@@ -8078,6 +10178,26 @@
           <t>2015-01-29T23:38:44</t>
         </is>
       </c>
+      <c r="Q106" t="inlineStr">
+        <is>
+          <t>PB15</t>
+        </is>
+      </c>
+      <c r="R106" t="inlineStr">
+        <is>
+          <t>PX05</t>
+        </is>
+      </c>
+      <c r="S106" t="inlineStr">
+        <is>
+          <t>2015-01-29T23:38:45</t>
+        </is>
+      </c>
+      <c r="T106" t="inlineStr">
+        <is>
+          <t>2015-01-29T23:38:47</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
@@ -8150,6 +10270,26 @@
           <t>2015-01-30T11:55:15</t>
         </is>
       </c>
+      <c r="Q107" t="inlineStr">
+        <is>
+          <t>MT02</t>
+        </is>
+      </c>
+      <c r="R107" t="inlineStr">
+        <is>
+          <t>VA05</t>
+        </is>
+      </c>
+      <c r="S107" t="inlineStr">
+        <is>
+          <t>2015-01-30T11:55:16</t>
+        </is>
+      </c>
+      <c r="T107" t="inlineStr">
+        <is>
+          <t>2015-01-30T11:55:19</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
@@ -8222,6 +10362,26 @@
           <t>2015-02-03T18:48:27</t>
         </is>
       </c>
+      <c r="Q108" t="inlineStr">
+        <is>
+          <t>PB15</t>
+        </is>
+      </c>
+      <c r="R108" t="inlineStr">
+        <is>
+          <t>PB03</t>
+        </is>
+      </c>
+      <c r="S108" t="inlineStr">
+        <is>
+          <t>2015-02-03T18:48:28</t>
+        </is>
+      </c>
+      <c r="T108" t="inlineStr">
+        <is>
+          <t>2015-02-03T18:48:33</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
@@ -8294,6 +10454,26 @@
           <t>2015-02-17T21:21:57</t>
         </is>
       </c>
+      <c r="Q109" t="inlineStr">
+        <is>
+          <t>PB03</t>
+        </is>
+      </c>
+      <c r="R109" t="inlineStr">
+        <is>
+          <t>PB06</t>
+        </is>
+      </c>
+      <c r="S109" t="inlineStr">
+        <is>
+          <t>2015-02-17T21:21:58</t>
+        </is>
+      </c>
+      <c r="T109" t="inlineStr">
+        <is>
+          <t>2015-02-17T21:21:58</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
@@ -8366,6 +10546,26 @@
           <t>2015-02-17T22:11:57</t>
         </is>
       </c>
+      <c r="Q110" t="inlineStr">
+        <is>
+          <t>PB04</t>
+        </is>
+      </c>
+      <c r="R110" t="inlineStr">
+        <is>
+          <t>PB01</t>
+        </is>
+      </c>
+      <c r="S110" t="inlineStr">
+        <is>
+          <t>2015-02-17T22:11:57</t>
+        </is>
+      </c>
+      <c r="T110" t="inlineStr">
+        <is>
+          <t>2015-02-17T22:11:59</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="n">
@@ -8438,6 +10638,26 @@
           <t>2015-02-19T16:18:51</t>
         </is>
       </c>
+      <c r="Q111" t="inlineStr">
+        <is>
+          <t>VA01</t>
+        </is>
+      </c>
+      <c r="R111" t="inlineStr">
+        <is>
+          <t>VA03</t>
+        </is>
+      </c>
+      <c r="S111" t="inlineStr">
+        <is>
+          <t>2015-02-19T16:18:51</t>
+        </is>
+      </c>
+      <c r="T111" t="inlineStr">
+        <is>
+          <t>2015-02-19T16:18:52</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
@@ -8510,6 +10730,26 @@
           <t>2015-03-02T08:28:47</t>
         </is>
       </c>
+      <c r="Q112" t="inlineStr">
+        <is>
+          <t>AC01</t>
+        </is>
+      </c>
+      <c r="R112" t="inlineStr">
+        <is>
+          <t>AC05</t>
+        </is>
+      </c>
+      <c r="S112" t="inlineStr">
+        <is>
+          <t>2015-03-02T08:28:51</t>
+        </is>
+      </c>
+      <c r="T112" t="inlineStr">
+        <is>
+          <t>2015-03-02T08:28:57</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="n">
@@ -8582,6 +10822,26 @@
           <t>2015-03-26T22:30:35</t>
         </is>
       </c>
+      <c r="Q113" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="R113" t="inlineStr">
+        <is>
+          <t>TA01</t>
+        </is>
+      </c>
+      <c r="S113" t="inlineStr">
+        <is>
+          <t>2015-03-26T22:30:36</t>
+        </is>
+      </c>
+      <c r="T113" t="inlineStr">
+        <is>
+          <t>2015-03-26T22:30:37</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
@@ -8654,6 +10914,26 @@
           <t>2015-03-30T12:24:14</t>
         </is>
       </c>
+      <c r="Q114" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="R114" t="inlineStr">
+        <is>
+          <t>PSGCX</t>
+        </is>
+      </c>
+      <c r="S114" t="inlineStr">
+        <is>
+          <t>2015-03-30T12:24:15</t>
+        </is>
+      </c>
+      <c r="T114" t="inlineStr">
+        <is>
+          <t>2015-03-30T12:24:16</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
@@ -8726,6 +11006,26 @@
           <t>2015-04-07T21:16:35</t>
         </is>
       </c>
+      <c r="Q115" t="inlineStr">
+        <is>
+          <t>IN41</t>
+        </is>
+      </c>
+      <c r="R115" t="inlineStr">
+        <is>
+          <t>CO05</t>
+        </is>
+      </c>
+      <c r="S115" t="inlineStr">
+        <is>
+          <t>2015-04-07T21:16:35</t>
+        </is>
+      </c>
+      <c r="T115" t="inlineStr">
+        <is>
+          <t>2015-04-07T21:16:36</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -8798,6 +11098,26 @@
           <t>2015-04-12T09:42:04</t>
         </is>
       </c>
+      <c r="Q116" t="inlineStr">
+        <is>
+          <t>PB15</t>
+        </is>
+      </c>
+      <c r="R116" t="inlineStr">
+        <is>
+          <t>PX05</t>
+        </is>
+      </c>
+      <c r="S116" t="inlineStr">
+        <is>
+          <t>2015-04-12T09:42:06</t>
+        </is>
+      </c>
+      <c r="T116" t="inlineStr">
+        <is>
+          <t>2015-04-12T09:42:06</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -8870,6 +11190,26 @@
           <t>2015-04-14T01:59:41</t>
         </is>
       </c>
+      <c r="Q117" t="inlineStr">
+        <is>
+          <t>PB10</t>
+        </is>
+      </c>
+      <c r="R117" t="inlineStr">
+        <is>
+          <t>PX06</t>
+        </is>
+      </c>
+      <c r="S117" t="inlineStr">
+        <is>
+          <t>2015-04-14T01:59:43</t>
+        </is>
+      </c>
+      <c r="T117" t="inlineStr">
+        <is>
+          <t>2015-04-14T01:59:43</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
@@ -8942,6 +11282,26 @@
           <t>2015-05-12T05:50:22</t>
         </is>
       </c>
+      <c r="Q118" t="inlineStr">
+        <is>
+          <t>PB07</t>
+        </is>
+      </c>
+      <c r="R118" t="inlineStr">
+        <is>
+          <t>PB10</t>
+        </is>
+      </c>
+      <c r="S118" t="inlineStr">
+        <is>
+          <t>2015-05-12T05:50:24</t>
+        </is>
+      </c>
+      <c r="T118" t="inlineStr">
+        <is>
+          <t>2015-05-12T05:50:27</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -9014,6 +11374,26 @@
           <t>2015-05-14T09:09:31</t>
         </is>
       </c>
+      <c r="Q119" t="inlineStr">
+        <is>
+          <t>HMBCX</t>
+        </is>
+      </c>
+      <c r="R119" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="S119" t="inlineStr">
+        <is>
+          <t>2015-05-14T09:09:34</t>
+        </is>
+      </c>
+      <c r="T119" t="inlineStr">
+        <is>
+          <t>2015-05-14T09:09:34</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
@@ -9086,6 +11466,26 @@
           <t>2015-05-14T16:37:04</t>
         </is>
       </c>
+      <c r="Q120" t="inlineStr">
+        <is>
+          <t>IN41</t>
+        </is>
+      </c>
+      <c r="R120" t="inlineStr">
+        <is>
+          <t>TLL</t>
+        </is>
+      </c>
+      <c r="S120" t="inlineStr">
+        <is>
+          <t>2015-05-14T16:37:04</t>
+        </is>
+      </c>
+      <c r="T120" t="inlineStr">
+        <is>
+          <t>2015-05-14T16:37:07</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
@@ -9158,6 +11558,26 @@
           <t>2015-06-01T04:28:04</t>
         </is>
       </c>
+      <c r="Q121" t="inlineStr">
+        <is>
+          <t>PB15</t>
+        </is>
+      </c>
+      <c r="R121" t="inlineStr">
+        <is>
+          <t>PX05</t>
+        </is>
+      </c>
+      <c r="S121" t="inlineStr">
+        <is>
+          <t>2015-06-01T04:28:05</t>
+        </is>
+      </c>
+      <c r="T121" t="inlineStr">
+        <is>
+          <t>2015-06-01T04:28:08</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
@@ -9230,6 +11650,26 @@
           <t>2015-06-11T12:04:39</t>
         </is>
       </c>
+      <c r="Q122" t="inlineStr">
+        <is>
+          <t>TA01</t>
+        </is>
+      </c>
+      <c r="R122" t="inlineStr">
+        <is>
+          <t>PB03</t>
+        </is>
+      </c>
+      <c r="S122" t="inlineStr">
+        <is>
+          <t>2015-06-11T12:04:41</t>
+        </is>
+      </c>
+      <c r="T122" t="inlineStr">
+        <is>
+          <t>2015-06-11T12:04:41</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
@@ -9302,6 +11742,26 @@
           <t>2015-07-12T05:36:32</t>
         </is>
       </c>
+      <c r="Q123" t="inlineStr">
+        <is>
+          <t>CO04</t>
+        </is>
+      </c>
+      <c r="R123" t="inlineStr">
+        <is>
+          <t>MT02</t>
+        </is>
+      </c>
+      <c r="S123" t="inlineStr">
+        <is>
+          <t>2015-07-12T05:36:33</t>
+        </is>
+      </c>
+      <c r="T123" t="inlineStr">
+        <is>
+          <t>2015-07-12T05:36:34</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
@@ -9374,6 +11834,26 @@
           <t>2015-07-25T01:58:41</t>
         </is>
       </c>
+      <c r="Q124" t="inlineStr">
+        <is>
+          <t>PX03</t>
+        </is>
+      </c>
+      <c r="R124" t="inlineStr">
+        <is>
+          <t>PB11</t>
+        </is>
+      </c>
+      <c r="S124" t="inlineStr">
+        <is>
+          <t>2015-07-25T01:58:44</t>
+        </is>
+      </c>
+      <c r="T124" t="inlineStr">
+        <is>
+          <t>2015-07-25T01:58:45</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
@@ -9446,6 +11926,26 @@
           <t>2015-08-01T18:11:12</t>
         </is>
       </c>
+      <c r="Q125" t="inlineStr">
+        <is>
+          <t>PB05</t>
+        </is>
+      </c>
+      <c r="R125" t="inlineStr">
+        <is>
+          <t>PB06</t>
+        </is>
+      </c>
+      <c r="S125" t="inlineStr">
+        <is>
+          <t>2015-08-01T18:11:12</t>
+        </is>
+      </c>
+      <c r="T125" t="inlineStr">
+        <is>
+          <t>2015-08-01T18:11:14</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
@@ -9516,6 +12016,26 @@
       <c r="P126" t="inlineStr">
         <is>
           <t>2015-08-06T07:31:22</t>
+        </is>
+      </c>
+      <c r="Q126" t="inlineStr">
+        <is>
+          <t>IN40</t>
+        </is>
+      </c>
+      <c r="R126" t="inlineStr">
+        <is>
+          <t>CO03</t>
+        </is>
+      </c>
+      <c r="S126" t="inlineStr">
+        <is>
+          <t>2015-08-06T07:31:22</t>
+        </is>
+      </c>
+      <c r="T126" t="inlineStr">
+        <is>
+          <t>2015-08-06T07:31:23</t>
         </is>
       </c>
     </row>

</xml_diff>